<commit_message>
added poisson calculation in main.db
</commit_message>
<xml_diff>
--- a/myodds.xlsx
+++ b/myodds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="435">
   <si>
     <t>Bookmaker's odds</t>
   </si>
@@ -1827,8 +1827,8 @@
   <dimension ref="A1:W409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U187" sqref="U187"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U196" sqref="U196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17010,15 +17010,19 @@
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A187" s="9"/>
-      <c r="B187" s="9"/>
-      <c r="C187" s="16" t="e">
+      <c r="A187" s="9">
+        <v>0.22</v>
+      </c>
+      <c r="B187" s="9">
+        <v>0.78</v>
+      </c>
+      <c r="C187" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D187" s="17" t="e">
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="D187" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1.2820512820512819</v>
       </c>
       <c r="E187" s="12">
         <v>3.0357331084642114E-2</v>
@@ -17027,13 +17031,13 @@
         <f t="shared" si="34"/>
         <v>1.0303573310846421</v>
       </c>
-      <c r="G187" s="7" t="e">
+      <c r="G187" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H187" s="7" t="e">
+        <v>4.4115322018135323</v>
+      </c>
+      <c r="H187" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>1.2442783133320217</v>
       </c>
       <c r="I187">
         <v>1.79</v>
@@ -17057,13 +17061,13 @@
         <f t="shared" si="52"/>
         <v>0.45780051150895146</v>
       </c>
-      <c r="O187" s="15" t="e">
+      <c r="O187" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P187" s="15" t="e">
+        <v>0.40575471698113202</v>
+      </c>
+      <c r="P187" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.7037988826815644</v>
       </c>
       <c r="Q187" t="s">
         <v>248</v>
@@ -17074,20 +17078,30 @@
       <c r="S187" t="s">
         <v>291</v>
       </c>
+      <c r="T187" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="U187" s="8" t="s">
+        <v>307</v>
+      </c>
       <c r="V187" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9"/>
-      <c r="C188" s="16" t="e">
+      <c r="A188" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="B188" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C188" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D188" s="17" t="e">
+        <v>1.25</v>
+      </c>
+      <c r="D188" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="E188" s="12">
         <v>3.4313725490195957E-2</v>
@@ -17096,13 +17110,13 @@
         <f t="shared" si="34"/>
         <v>1.034313725490196</v>
       </c>
-      <c r="G188" s="7" t="e">
+      <c r="G188" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H188" s="7" t="e">
+        <v>1.2085308056872039</v>
+      </c>
+      <c r="H188" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>4.8341232227488158</v>
       </c>
       <c r="I188">
         <v>1.5</v>
@@ -17126,13 +17140,13 @@
         <f t="shared" si="52"/>
         <v>0.35545023696682471</v>
       </c>
-      <c r="O188" s="15" t="e">
+      <c r="O188" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P188" s="15" t="e">
+        <v>1.2411764705882351</v>
+      </c>
+      <c r="P188" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>0.56266666666666665</v>
       </c>
       <c r="Q188" t="s">
         <v>226</v>
@@ -17143,20 +17157,30 @@
       <c r="S188" t="s">
         <v>291</v>
       </c>
+      <c r="T188" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="U188" s="8" t="s">
+        <v>300</v>
+      </c>
       <c r="V188" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A189" s="9"/>
-      <c r="B189" s="9"/>
-      <c r="C189" s="16" t="e">
+      <c r="A189" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="B189" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="C189" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D189" s="17" t="e">
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="D189" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1.9230769230769229</v>
       </c>
       <c r="E189" s="12">
         <v>2.8345418589321048E-2</v>
@@ -17165,13 +17189,13 @@
         <f t="shared" si="34"/>
         <v>1.028345418589321</v>
       </c>
-      <c r="G189" s="7" t="e">
+      <c r="G189" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H189" s="7" t="e">
+        <v>2.0259081196581197</v>
+      </c>
+      <c r="H189" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>1.8700690335305719</v>
       </c>
       <c r="I189">
         <v>1.85</v>
@@ -17195,13 +17219,13 @@
         <f t="shared" si="52"/>
         <v>0.47435897435897439</v>
       </c>
-      <c r="O189" s="15" t="e">
+      <c r="O189" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P189" s="15" t="e">
+        <v>0.91317073170731711</v>
+      </c>
+      <c r="P189" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.0962162162162161</v>
       </c>
       <c r="Q189" t="s">
         <v>228</v>
@@ -17212,20 +17236,30 @@
       <c r="S189" t="s">
         <v>292</v>
       </c>
+      <c r="T189" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U189" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="V189" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A190" s="9"/>
-      <c r="B190" s="9"/>
-      <c r="C190" s="16" t="e">
+      <c r="A190" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B190" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="C190" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D190" s="17" t="e">
+        <v>1.7857142857142856</v>
+      </c>
+      <c r="D190" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="E190" s="12">
         <v>2.861071447458885E-2</v>
@@ -17234,13 +17268,13 @@
         <f t="shared" si="34"/>
         <v>1.0286107144745888</v>
       </c>
-      <c r="G190" s="7" t="e">
+      <c r="G190" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H190" s="7" t="e">
+        <v>1.7360448035255232</v>
+      </c>
+      <c r="H190" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>2.2095115681233937</v>
       </c>
       <c r="I190">
         <v>1.91</v>
@@ -17264,13 +17298,13 @@
         <f t="shared" si="52"/>
         <v>0.49100257069408743</v>
       </c>
-      <c r="O190" s="15" t="e">
+      <c r="O190" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P190" s="15" t="e">
+        <v>1.1002020202020202</v>
+      </c>
+      <c r="P190" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>0.8961256544502616</v>
       </c>
       <c r="Q190" t="s">
         <v>251</v>
@@ -17281,20 +17315,30 @@
       <c r="S190" t="s">
         <v>292</v>
       </c>
+      <c r="T190" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U190" s="8" t="s">
+        <v>316</v>
+      </c>
       <c r="V190" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A191" s="9"/>
-      <c r="B191" s="9"/>
-      <c r="C191" s="16" t="e">
+      <c r="A191" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="B191" s="9">
+        <v>0.47</v>
+      </c>
+      <c r="C191" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D191" s="17" t="e">
+        <v>1.8867924528301885</v>
+      </c>
+      <c r="D191" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>2.1276595744680851</v>
       </c>
       <c r="E191" s="12">
         <v>3.5940803382663811E-2</v>
@@ -17303,13 +17347,13 @@
         <f t="shared" si="34"/>
         <v>1.0359408033826638</v>
       </c>
-      <c r="G191" s="7" t="e">
+      <c r="G191" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H191" s="7" t="e">
+        <v>1.8213323065075084</v>
+      </c>
+      <c r="H191" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>2.053842813721233</v>
       </c>
       <c r="I191">
         <v>1.72</v>
@@ -17333,13 +17377,13 @@
         <f t="shared" si="52"/>
         <v>0.43877551020408162</v>
       </c>
-      <c r="O191" s="15" t="e">
+      <c r="O191" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P191" s="15" t="e">
+        <v>0.94436363636363652</v>
+      </c>
+      <c r="P191" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.0711627906976746</v>
       </c>
       <c r="Q191" t="s">
         <v>257</v>
@@ -17350,20 +17394,30 @@
       <c r="S191" t="s">
         <v>292</v>
       </c>
+      <c r="T191" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U191" s="8" t="s">
+        <v>316</v>
+      </c>
       <c r="V191" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A192" s="9"/>
-      <c r="B192" s="9"/>
-      <c r="C192" s="16" t="e">
+      <c r="A192" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="B192" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="C192" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D192" s="17" t="e">
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="D192" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1.5625</v>
       </c>
       <c r="E192" s="12">
         <v>2.8001534330648337E-2</v>
@@ -17372,13 +17426,13 @@
         <f t="shared" si="34"/>
         <v>1.0280015343306483</v>
       </c>
-      <c r="G192" s="7" t="e">
+      <c r="G192" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H192" s="7" t="e">
+        <v>2.7021144278606961</v>
+      </c>
+      <c r="H192" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>1.5199393656716416</v>
       </c>
       <c r="I192">
         <v>2.37</v>
@@ -17402,13 +17456,13 @@
         <f t="shared" si="52"/>
         <v>0.58955223880597019</v>
       </c>
-      <c r="O192" s="15" t="e">
+      <c r="O192" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P192" s="15" t="e">
+        <v>0.87709090909090925</v>
+      </c>
+      <c r="P192" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.0855696202531646</v>
       </c>
       <c r="Q192" t="s">
         <v>331</v>
@@ -17419,20 +17473,30 @@
       <c r="S192" t="s">
         <v>349</v>
       </c>
+      <c r="T192" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U192" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="V192" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="193" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A193" s="9"/>
-      <c r="B193" s="9"/>
-      <c r="C193" s="16" t="e">
+      <c r="A193" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="B193" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="C193" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D193" s="17" t="e">
+        <v>1.5625</v>
+      </c>
+      <c r="D193" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>2.7777777777777777</v>
       </c>
       <c r="E193" s="12">
         <v>3.0163599182004175E-2</v>
@@ -17441,13 +17505,13 @@
         <f t="shared" si="34"/>
         <v>1.0301635991820042</v>
       </c>
-      <c r="G193" s="7" t="e">
+      <c r="G193" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H193" s="7" t="e">
+        <v>1.5167493796526053</v>
+      </c>
+      <c r="H193" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>2.6964433416046316</v>
       </c>
       <c r="I193">
         <v>1.63</v>
@@ -17471,13 +17535,13 @@
         <f t="shared" si="52"/>
         <v>0.40446650124069478</v>
       </c>
-      <c r="O193" s="15" t="e">
+      <c r="O193" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P193" s="15" t="e">
+        <v>1.0746666666666667</v>
+      </c>
+      <c r="P193" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>0.89006134969325157</v>
       </c>
       <c r="Q193" t="s">
         <v>360</v>
@@ -17488,20 +17552,30 @@
       <c r="S193" t="s">
         <v>349</v>
       </c>
+      <c r="T193" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U193" s="8" t="s">
+        <v>304</v>
+      </c>
       <c r="V193" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="194" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A194" s="9"/>
-      <c r="B194" s="9"/>
-      <c r="C194" s="16" t="e">
+      <c r="A194" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="B194" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="C194" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D194" s="17" t="e">
+        <v>2.5641025641025639</v>
+      </c>
+      <c r="D194" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1.639344262295082</v>
       </c>
       <c r="E194" s="12">
         <v>2.79347143753923E-2</v>
@@ -17510,13 +17584,13 @@
         <f t="shared" ref="F194:F257" si="55">(E194/100%) + 1</f>
         <v>1.0279347143753923</v>
       </c>
-      <c r="G194" s="7" t="e">
+      <c r="G194" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H194" s="7" t="e">
+        <v>2.4944216089254256</v>
+      </c>
+      <c r="H194" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>1.594794143411338</v>
       </c>
       <c r="I194">
         <v>2.16</v>
@@ -17540,13 +17614,13 @@
         <f t="shared" si="52"/>
         <v>0.54961832061068705</v>
       </c>
-      <c r="O194" s="15" t="e">
+      <c r="O194" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P194" s="15" t="e">
+        <v>0.86593220338983057</v>
+      </c>
+      <c r="P194" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.109861111111111</v>
       </c>
       <c r="Q194" t="s">
         <v>361</v>
@@ -17557,20 +17631,30 @@
       <c r="S194" t="s">
         <v>349</v>
       </c>
+      <c r="T194" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="U194" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="V194" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="195" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A195" s="9"/>
-      <c r="B195" s="9"/>
-      <c r="C195" s="16" t="e">
+      <c r="A195" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="B195" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C195" s="16">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D195" s="17" t="e">
+        <v>2.2727272727272729</v>
+      </c>
+      <c r="D195" s="17">
         <f t="shared" si="46"/>
-        <v>#DIV/0!</v>
+        <v>1.7857142857142856</v>
       </c>
       <c r="E195" s="12">
         <v>2.9539874871307603E-2</v>
@@ -17579,13 +17663,13 @@
         <f t="shared" si="55"/>
         <v>1.0295398748713076</v>
       </c>
-      <c r="G195" s="7" t="e">
+      <c r="G195" s="7">
         <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H195" s="7" t="e">
+        <v>2.2075174825174826</v>
+      </c>
+      <c r="H195" s="7">
         <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
+        <v>1.7344780219780218</v>
       </c>
       <c r="I195">
         <v>1.83</v>
@@ -17609,13 +17693,13 @@
         <f t="shared" si="52"/>
         <v>0.46923076923076917</v>
       </c>
-      <c r="O195" s="15" t="e">
+      <c r="O195" s="15">
         <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P195" s="15" t="e">
+        <v>0.82898550724637676</v>
+      </c>
+      <c r="P195" s="15">
         <f t="shared" si="54"/>
-        <v>#DIV/0!</v>
+        <v>1.1934426229508197</v>
       </c>
       <c r="Q195" t="s">
         <v>344</v>
@@ -17625,6 +17709,12 @@
       </c>
       <c r="S195" t="s">
         <v>349</v>
+      </c>
+      <c r="T195" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="U195" s="8" t="s">
+        <v>305</v>
       </c>
       <c r="V195" t="s">
         <v>432</v>
@@ -27616,7 +27706,7 @@
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A186" sqref="A186:XFD186"/>
+      <selection pane="bottomLeft" activeCell="A195" sqref="A195:C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47495,20 +47585,26 @@
       </c>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A187" s="9"/>
-      <c r="B187" s="9"/>
-      <c r="C187" s="9"/>
-      <c r="D187" s="3" t="e">
+      <c r="A187" s="9">
+        <v>0.37129934086969912</v>
+      </c>
+      <c r="B187" s="9">
+        <v>0.34884400310672858</v>
+      </c>
+      <c r="C187" s="9">
+        <v>0.2798566525160639</v>
+      </c>
+      <c r="D187" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E187" s="4" t="e">
+        <v>2.6932447487186146</v>
+      </c>
+      <c r="E187" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F187" s="13" t="e">
+        <v>2.8666108377791168</v>
+      </c>
+      <c r="F187" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>3.573257919758043</v>
       </c>
       <c r="G187" s="12">
         <v>2.3510032943995007E-2</v>
@@ -47517,17 +47613,17 @@
         <f t="shared" si="53"/>
         <v>1.023510032943995</v>
       </c>
-      <c r="I187" s="5" t="e">
+      <c r="I187" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J187" s="5" t="e">
+        <v>2.6313808971386852</v>
+      </c>
+      <c r="J187" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K187" s="5" t="e">
+        <v>2.8007647658652446</v>
+      </c>
+      <c r="K187" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>3.4911801592017873</v>
       </c>
       <c r="L187">
         <v>3.6</v>
@@ -47562,17 +47658,17 @@
         <f t="shared" si="80"/>
         <v>0.46525237746891013</v>
       </c>
-      <c r="U187" t="e">
+      <c r="U187">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V187" t="e">
+        <v>1.3681029621802656</v>
+      </c>
+      <c r="V187">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W187" t="e">
+        <v>1.3246382006858273</v>
+      </c>
+      <c r="W187">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>0.60151579243625675</v>
       </c>
       <c r="X187" t="s">
         <v>248</v>
@@ -47588,20 +47684,26 @@
       </c>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9"/>
-      <c r="C188" s="9"/>
-      <c r="D188" s="3" t="e">
+      <c r="A188" s="9">
+        <v>0.23463255043551384</v>
+      </c>
+      <c r="B188" s="9">
+        <v>0.18073184744129223</v>
+      </c>
+      <c r="C188" s="9">
+        <v>0.58453651640354176</v>
+      </c>
+      <c r="D188" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E188" s="4" t="e">
+        <v>4.2619832505926709</v>
+      </c>
+      <c r="E188" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F188" s="13" t="e">
+        <v>5.5330591379299303</v>
+      </c>
+      <c r="F188" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>1.7107571074475663</v>
       </c>
       <c r="G188" s="12">
         <v>2.2604823394235973E-2</v>
@@ -47610,17 +47712,17 @@
         <f t="shared" si="53"/>
         <v>1.022604823394236</v>
       </c>
-      <c r="I188" s="5" t="e">
+      <c r="I188" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J188" s="5" t="e">
+        <v>4.1677715116248626</v>
+      </c>
+      <c r="J188" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K188" s="5" t="e">
+        <v>5.4107500877656411</v>
+      </c>
+      <c r="K188" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>1.6729405810635736</v>
       </c>
       <c r="L188">
         <v>2.92</v>
@@ -47655,17 +47757,17 @@
         <f t="shared" si="80"/>
         <v>0.4143622285614485</v>
       </c>
-      <c r="U188" t="e">
+      <c r="U188">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V188" t="e">
+        <v>0.70061422317789157</v>
+      </c>
+      <c r="V188">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W188" t="e">
+        <v>0.72078730984422479</v>
+      </c>
+      <c r="W188">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>1.4106896722534088</v>
       </c>
       <c r="X188" t="s">
         <v>226</v>
@@ -47681,20 +47783,26 @@
       </c>
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A189" s="9"/>
-      <c r="B189" s="9"/>
-      <c r="C189" s="9"/>
-      <c r="D189" s="3" t="e">
+      <c r="A189" s="9">
+        <v>0.64022647314302727</v>
+      </c>
+      <c r="B189" s="9">
+        <v>0.21705378938130396</v>
+      </c>
+      <c r="C189" s="9">
+        <v>0.14271536689544242</v>
+      </c>
+      <c r="D189" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E189" s="4" t="e">
+        <v>1.56194728264009</v>
+      </c>
+      <c r="E189" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F189" s="13" t="e">
+        <v>4.6071529220956116</v>
+      </c>
+      <c r="F189" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>7.0069539234175817</v>
       </c>
       <c r="G189" s="12">
         <v>2.9655095309967017E-2</v>
@@ -47703,17 +47811,17 @@
         <f t="shared" si="53"/>
         <v>1.029655095309967</v>
       </c>
-      <c r="I189" s="5" t="e">
+      <c r="I189" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J189" s="5" t="e">
+        <v>1.5169616406063449</v>
+      </c>
+      <c r="J189" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K189" s="5" t="e">
+        <v>4.4744623156637475</v>
+      </c>
+      <c r="K189" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>6.8051466508872185</v>
       </c>
       <c r="L189">
         <v>2</v>
@@ -47748,17 +47856,17 @@
         <f t="shared" si="80"/>
         <v>0.24159179130812458</v>
       </c>
-      <c r="U189" t="e">
+      <c r="U189">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V189" t="e">
+        <v>1.3184249004480957</v>
+      </c>
+      <c r="V189">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W189" t="e">
+        <v>0.79562632308635395</v>
+      </c>
+      <c r="W189">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>0.59072937090575317</v>
       </c>
       <c r="X189" t="s">
         <v>228</v>
@@ -47774,20 +47882,26 @@
       </c>
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A190" s="9"/>
-      <c r="B190" s="9"/>
-      <c r="C190" s="9"/>
-      <c r="D190" s="3" t="e">
+      <c r="A190" s="9">
+        <v>0.69437545673915368</v>
+      </c>
+      <c r="B190" s="9">
+        <v>0.18693221088767259</v>
+      </c>
+      <c r="C190" s="9">
+        <v>0.11867617256818047</v>
+      </c>
+      <c r="D190" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E190" s="4" t="e">
+        <v>1.4401430671183069</v>
+      </c>
+      <c r="E190" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F190" s="13" t="e">
+        <v>5.3495328346643225</v>
+      </c>
+      <c r="F190" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>8.4262912963888468</v>
       </c>
       <c r="G190" s="12">
         <v>2.6999982289286795E-2</v>
@@ -47796,17 +47910,17 @@
         <f t="shared" si="53"/>
         <v>1.0269999822892868</v>
       </c>
-      <c r="I190" s="5" t="e">
+      <c r="I190" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J190" s="5" t="e">
+        <v>1.4022814916783954</v>
+      </c>
+      <c r="J190" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K190" s="5" t="e">
+        <v>5.2088928207570877</v>
+      </c>
+      <c r="K190" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>8.2047628448890446</v>
       </c>
       <c r="L190">
         <v>3.19</v>
@@ -47841,17 +47955,17 @@
         <f t="shared" si="80"/>
         <v>0.41970252209527914</v>
       </c>
-      <c r="U190" t="e">
+      <c r="U190">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V190" t="e">
+        <v>2.2748642258565921</v>
+      </c>
+      <c r="V190">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W190" t="e">
+        <v>0.67960699553911685</v>
+      </c>
+      <c r="W190">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>0.28276259093158151</v>
       </c>
       <c r="X190" t="s">
         <v>251</v>
@@ -47867,20 +47981,26 @@
       </c>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A191" s="9"/>
-      <c r="B191" s="9"/>
-      <c r="C191" s="9"/>
-      <c r="D191" s="3" t="e">
+      <c r="A191" s="9">
+        <v>0.78569468180377411</v>
+      </c>
+      <c r="B191" s="9">
+        <v>0.15203477560086567</v>
+      </c>
+      <c r="C191" s="9">
+        <v>6.2240492415554412E-2</v>
+      </c>
+      <c r="D191" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E191" s="4" t="e">
+        <v>1.2727590286143089</v>
+      </c>
+      <c r="E191" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F191" s="13" t="e">
+        <v>6.5774425360766351</v>
+      </c>
+      <c r="F191" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>16.066710933509448</v>
       </c>
       <c r="G191" s="12">
         <v>2.9844758948999184E-2</v>
@@ -47889,17 +48009,17 @@
         <f t="shared" si="53"/>
         <v>1.0298447589489992</v>
       </c>
-      <c r="I191" s="5" t="e">
+      <c r="I191" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J191" s="5" t="e">
+        <v>1.2358746476636091</v>
+      </c>
+      <c r="J191" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K191" s="5" t="e">
+        <v>6.3868291593668909</v>
+      </c>
+      <c r="K191" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>15.601099868592055</v>
       </c>
       <c r="L191">
         <v>1.67</v>
@@ -47934,17 +48054,17 @@
         <f t="shared" si="80"/>
         <v>0.18286631601608488</v>
       </c>
-      <c r="U191" t="e">
+      <c r="U191">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V191" t="e">
+        <v>1.3512697288168296</v>
+      </c>
+      <c r="V191">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W191" t="e">
+        <v>0.64507753334181939</v>
+      </c>
+      <c r="W191">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>0.34036061846447296</v>
       </c>
       <c r="X191" t="s">
         <v>257</v>
@@ -47960,20 +48080,26 @@
       </c>
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A192" s="9"/>
-      <c r="B192" s="9"/>
-      <c r="C192" s="9"/>
-      <c r="D192" s="3" t="e">
+      <c r="A192" s="9">
+        <v>0.60094847821193087</v>
+      </c>
+      <c r="B192" s="9">
+        <v>0.2552177012388635</v>
+      </c>
+      <c r="C192" s="9">
+        <v>0.14383314036308029</v>
+      </c>
+      <c r="D192" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E192" s="4" t="e">
+        <v>1.6640361632588065</v>
+      </c>
+      <c r="E192" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F192" s="13" t="e">
+        <v>3.9182235211188563</v>
+      </c>
+      <c r="F192" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>6.9525006370276285</v>
       </c>
       <c r="G192" s="12">
         <v>2.520991848574905E-2</v>
@@ -47982,17 +48108,17 @@
         <f t="shared" si="53"/>
         <v>1.025209918485749</v>
       </c>
-      <c r="I192" s="5" t="e">
+      <c r="I192" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J192" s="5" t="e">
+        <v>1.6231175033076286</v>
+      </c>
+      <c r="J192" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K192" s="5" t="e">
+        <v>3.8218743795476864</v>
+      </c>
+      <c r="K192" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>6.7815386016715289</v>
       </c>
       <c r="L192">
         <v>1.63</v>
@@ -48027,17 +48153,17 @@
         <f t="shared" si="80"/>
         <v>0.13796463841186254</v>
       </c>
-      <c r="U192" t="e">
+      <c r="U192">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V192" t="e">
+        <v>1.0042402947897155</v>
+      </c>
+      <c r="V192">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W192" t="e">
+        <v>0.96811135912789736</v>
+      </c>
+      <c r="W192">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>1.0425362760977828</v>
       </c>
       <c r="X192" t="s">
         <v>331</v>
@@ -48053,20 +48179,26 @@
       </c>
     </row>
     <row r="193" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A193" s="9"/>
-      <c r="B193" s="9"/>
-      <c r="C193" s="9"/>
-      <c r="D193" s="3" t="e">
+      <c r="A193" s="9">
+        <v>0.47791523624913868</v>
+      </c>
+      <c r="B193" s="9">
+        <v>0.22533944083901677</v>
+      </c>
+      <c r="C193" s="9">
+        <v>0.29674073680652535</v>
+      </c>
+      <c r="D193" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E193" s="4" t="e">
+        <v>2.0924212583143027</v>
+      </c>
+      <c r="E193" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F193" s="13" t="e">
+        <v>4.4377495403230505</v>
+      </c>
+      <c r="F193" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>3.3699451270554706</v>
       </c>
       <c r="G193" s="12">
         <v>2.2740349867345966E-2</v>
@@ -48075,17 +48207,17 @@
         <f t="shared" si="53"/>
         <v>1.022740349867346</v>
       </c>
-      <c r="I193" s="5" t="e">
+      <c r="I193" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J193" s="5" t="e">
+        <v>2.0458968481938737</v>
+      </c>
+      <c r="J193" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K193" s="5" t="e">
+        <v>4.3390774020978506</v>
+      </c>
+      <c r="K193" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>3.2950153257301009</v>
       </c>
       <c r="L193">
         <v>2.1800000000000002</v>
@@ -48120,17 +48252,17 @@
         <f t="shared" si="80"/>
         <v>0.2850627625498377</v>
       </c>
-      <c r="U193" t="e">
+      <c r="U193">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V193" t="e">
+        <v>1.0655473671238671</v>
+      </c>
+      <c r="V193">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W193" t="e">
+        <v>0.84580192052477188</v>
+      </c>
+      <c r="W193">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>1.0409663266862013</v>
       </c>
       <c r="X193" t="s">
         <v>360</v>
@@ -48146,20 +48278,26 @@
       </c>
     </row>
     <row r="194" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A194" s="9"/>
-      <c r="B194" s="9"/>
-      <c r="C194" s="9"/>
-      <c r="D194" s="3" t="e">
+      <c r="A194" s="9">
+        <v>0.70368336387766373</v>
+      </c>
+      <c r="B194" s="9">
+        <v>0.21055529732355346</v>
+      </c>
+      <c r="C194" s="9">
+        <v>8.5758318025254424E-2</v>
+      </c>
+      <c r="D194" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E194" s="4" t="e">
+        <v>1.4210937068193235</v>
+      </c>
+      <c r="E194" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F194" s="13" t="e">
+        <v>4.7493461941417348</v>
+      </c>
+      <c r="F194" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>11.660676457128233</v>
       </c>
       <c r="G194" s="12">
         <v>2.5570618145352775E-2</v>
@@ -48168,17 +48306,17 @@
         <f t="shared" ref="H194:H257" si="84">(G194/100%) + 1</f>
         <v>1.0255706181453528</v>
       </c>
-      <c r="I194" s="5" t="e">
+      <c r="I194" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J194" s="5" t="e">
+        <v>1.3856614860800485</v>
+      </c>
+      <c r="J194" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K194" s="5" t="e">
+        <v>4.6309304401977478</v>
+      </c>
+      <c r="K194" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>11.369940061480564</v>
       </c>
       <c r="L194">
         <v>1.85</v>
@@ -48213,17 +48351,17 @@
         <f t="shared" si="80"/>
         <v>0.19980879830338752</v>
       </c>
-      <c r="U194" t="e">
+      <c r="U194">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V194" t="e">
+        <v>1.3351024175706412</v>
+      </c>
+      <c r="V194">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W194" t="e">
+        <v>0.77090339535472607</v>
+      </c>
+      <c r="W194">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>0.42920191079393771</v>
       </c>
       <c r="X194" t="s">
         <v>361</v>
@@ -48239,20 +48377,26 @@
       </c>
     </row>
     <row r="195" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A195" s="9"/>
-      <c r="B195" s="9"/>
-      <c r="C195" s="9"/>
-      <c r="D195" s="3" t="e">
+      <c r="A195" s="9">
+        <v>0.14233193326741073</v>
+      </c>
+      <c r="B195" s="9">
+        <v>0.22849422328188518</v>
+      </c>
+      <c r="C195" s="9">
+        <v>0.62917141647687258</v>
+      </c>
+      <c r="D195" s="3">
         <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E195" s="4" t="e">
+        <v>7.0258302339027292</v>
+      </c>
+      <c r="E195" s="4">
         <f t="shared" si="70"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F195" s="13" t="e">
+        <v>4.3764782568106133</v>
+      </c>
+      <c r="F195" s="13">
         <f t="shared" si="71"/>
-        <v>#DIV/0!</v>
+        <v>1.5893919746062695</v>
       </c>
       <c r="G195" s="12">
         <v>2.7676672623270449E-2</v>
@@ -48261,17 +48405,17 @@
         <f t="shared" si="84"/>
         <v>1.0276766726232704</v>
       </c>
-      <c r="I195" s="5" t="e">
+      <c r="I195" s="5">
         <f t="shared" si="72"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J195" s="5" t="e">
+        <v>6.8366154658044715</v>
+      </c>
+      <c r="J195" s="5">
         <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K195" s="5" t="e">
+        <v>4.2586139915379384</v>
+      </c>
+      <c r="K195" s="5">
         <f t="shared" si="74"/>
-        <v>#DIV/0!</v>
+        <v>1.5465875765664234</v>
       </c>
       <c r="L195">
         <v>6.81</v>
@@ -48306,17 +48450,17 @@
         <f t="shared" si="80"/>
         <v>0.62376198477809619</v>
       </c>
-      <c r="U195" t="e">
+      <c r="U195">
         <f t="shared" si="81"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V195" t="e">
+        <v>0.99610692367625508</v>
+      </c>
+      <c r="V195">
         <f t="shared" si="82"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W195" t="e">
+        <v>0.97919182351017997</v>
+      </c>
+      <c r="W195">
         <f t="shared" si="83"/>
-        <v>#DIV/0!</v>
+        <v>1.0086722689596108</v>
       </c>
       <c r="X195" t="s">
         <v>344</v>

</xml_diff>